<commit_message>
Removed space that caused the error of the issue
</commit_message>
<xml_diff>
--- a/Tests/ShouldSucceed/Issue192.xlsx
+++ b/Tests/ShouldSucceed/Issue192.xlsx
@@ -37,10 +37,10 @@
     <t>[Auto]</t>
   </si>
   <si>
-    <t xml:space="preserve">Aantal </t>
-  </si>
-  <si>
     <t>vier</t>
+  </si>
+  <si>
+    <t>Aantal</t>
   </si>
 </sst>
 </file>
@@ -383,10 +383,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -404,7 +409,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -415,7 +420,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>

</xml_diff>